<commit_message>
Batty connector modified in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -772,7 +772,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -993,15 +993,15 @@
         <v>1</v>
       </c>
       <c r="C12" s="7">
-        <f>2.3/20</f>
-        <v>0.11499999999999999</v>
+        <f>0.99*G60/10</f>
+        <v>8.4494520000000004E-2</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" ref="D12:D33" si="4">B12*C12</f>
-        <v>0.11499999999999999</v>
+        <v>8.4494520000000004E-2</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -1754,7 +1754,7 @@
       </c>
       <c r="D59" s="14">
         <f>SUM(D2:D57)</f>
-        <v>86.033865426909117</v>
+        <v>86.003359946909114</v>
       </c>
       <c r="G59" t="s">
         <v>44</v>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="D61" s="16">
         <f>D59+D60</f>
-        <v>97.85204724509093</v>
+        <v>97.821541765090927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Right angle male pin header link modified in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1159,15 +1159,15 @@
         <v>1</v>
       </c>
       <c r="C21" s="7">
-        <f>0.99*G61/5</f>
-        <v>0.16898904000000001</v>
+        <f>3.17/10</f>
+        <v>0.317</v>
       </c>
       <c r="D21" s="8">
         <f t="shared" si="4"/>
-        <v>0.16898904000000001</v>
+        <v>0.317</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="D60" s="14">
         <f>SUM(D3:D58)</f>
-        <v>88.482854466909089</v>
+        <v>88.630865426909097</v>
       </c>
       <c r="G60" t="s">
         <v>40</v>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D62" s="16">
         <f>D60+D61</f>
-        <v>100.3010362850909</v>
+        <v>100.44904724509091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Link of lipo charger modified
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1768,11 +1768,11 @@
         <v>1</v>
       </c>
       <c r="C59" s="7">
-        <v>9.76</v>
+        <v>6.15</v>
       </c>
       <c r="D59" s="8">
         <f>B59*C59</f>
-        <v>9.76</v>
+        <v>6.15</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>18</v>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D61" s="14">
         <f>SUM(D3:D59)</f>
-        <v>87.56065280290909</v>
+        <v>83.95065280290909</v>
       </c>
       <c r="G61" t="s">
         <v>39</v>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="D63" s="16">
         <f>D61+D62</f>
-        <v>99.378834621090903</v>
+        <v>95.768834621090903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wheels modified in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -213,13 +213,13 @@
     <t>EXTRA CÁMARA</t>
   </si>
   <si>
-    <t>Complubot</t>
-  </si>
-  <si>
     <t>Resistencia 120k</t>
   </si>
   <si>
     <t>Tira de conectores macho extendida</t>
+  </si>
+  <si>
+    <t>TME</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -906,14 +906,15 @@
         <v>1</v>
       </c>
       <c r="C7" s="7">
-        <v>6.03</v>
+        <f>3.93*B7+7.9</f>
+        <v>11.83</v>
       </c>
       <c r="D7" s="8">
         <f>B7*C7</f>
-        <v>6.03</v>
+        <v>11.83</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1137,7 +1138,7 @@
     </row>
     <row r="20" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
@@ -1308,7 +1309,7 @@
     </row>
     <row r="29" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
@@ -1792,7 +1793,7 @@
       </c>
       <c r="D61" s="14">
         <f>SUM(D3:D59)</f>
-        <v>83.95065280290909</v>
+        <v>89.750652802909087</v>
       </c>
       <c r="G61" t="s">
         <v>39</v>
@@ -1818,7 +1819,7 @@
       </c>
       <c r="D63" s="16">
         <f>D61+D62</f>
-        <v>95.768834621090903</v>
+        <v>101.5688346210909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fw and hw folders added
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>Unidades</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Resistencia 82k</t>
-  </si>
-  <si>
-    <t>Resistencia 47k</t>
   </si>
   <si>
     <t>Pulsador</t>
@@ -778,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -815,7 +812,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -868,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="7">
-        <f>3.35*G62</f>
+        <f>3.35*G61</f>
         <v>2.8591580000000003</v>
       </c>
       <c r="D5" s="8">
@@ -900,7 +897,7 @@
     </row>
     <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
@@ -914,12 +911,12 @@
         <v>11.83</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6">
         <v>2</v>
@@ -930,7 +927,7 @@
     </row>
     <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="6">
         <v>6</v>
@@ -949,7 +946,7 @@
     </row>
     <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="6">
         <v>6</v>
@@ -968,7 +965,7 @@
     </row>
     <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="6">
         <v>2</v>
@@ -987,7 +984,7 @@
     </row>
     <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6">
         <v>4</v>
@@ -1012,11 +1009,11 @@
         <v>1</v>
       </c>
       <c r="C13" s="7">
-        <f>0.99*G62/10</f>
+        <f>0.99*G61/10</f>
         <v>8.4494520000000004E-2</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" ref="D13:D35" si="4">B13*C13</f>
+        <f t="shared" ref="D13:D34" si="4">B13*C13</f>
         <v>8.4494520000000004E-2</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1106,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="7">
-        <f>2.81*G62/10</f>
+        <f>2.81*G61/10</f>
         <v>0.23982787999999999</v>
       </c>
       <c r="D18" s="8">
@@ -1119,7 +1116,7 @@
     </row>
     <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
@@ -1138,7 +1135,7 @@
     </row>
     <row r="20" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
@@ -1214,13 +1211,13 @@
     </row>
     <row r="24" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="6">
         <v>3</v>
       </c>
       <c r="C24" s="7">
-        <f>0.99*G62/100</f>
+        <f>0.99*G61/100</f>
         <v>8.4494520000000014E-3</v>
       </c>
       <c r="D24" s="8">
@@ -1233,13 +1230,13 @@
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="6">
         <v>2</v>
       </c>
       <c r="C25" s="7">
-        <f>0.99*G62/100</f>
+        <f>0.99*G61/100</f>
         <v>8.4494520000000014E-3</v>
       </c>
       <c r="D25" s="8">
@@ -1255,15 +1252,15 @@
         <v>24</v>
       </c>
       <c r="B26" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C26" s="7">
-        <f>0.99*G62/100</f>
+        <f>0.99*G61/100</f>
         <v>8.4494520000000014E-3</v>
       </c>
       <c r="D26" s="8">
         <f t="shared" si="4"/>
-        <v>1.6898904000000003E-2</v>
+        <v>6.7595616000000011E-2</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>17</v>
@@ -1271,18 +1268,18 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C27" s="7">
-        <f>0.99*G62/100</f>
+        <f>0.99*G61/100</f>
         <v>8.4494520000000014E-3</v>
       </c>
       <c r="D27" s="8">
         <f t="shared" si="4"/>
-        <v>5.0696712000000005E-2</v>
+        <v>8.4494520000000014E-3</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>17</v>
@@ -1290,13 +1287,13 @@
     </row>
     <row r="28" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B28" s="6">
         <v>1</v>
       </c>
       <c r="C28" s="7">
-        <f>0.99*G62/100</f>
+        <f>0.99*G61/100</f>
         <v>8.4494520000000014E-3</v>
       </c>
       <c r="D28" s="8">
@@ -1309,13 +1306,13 @@
     </row>
     <row r="29" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
       </c>
       <c r="C29" s="7">
-        <f>0.99*G62/100</f>
+        <f>0.99*G61/100</f>
         <v>8.4494520000000014E-3</v>
       </c>
       <c r="D29" s="8">
@@ -1328,18 +1325,18 @@
     </row>
     <row r="30" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
       </c>
       <c r="C30" s="7">
-        <f>0.99*G62/100</f>
-        <v>8.4494520000000014E-3</v>
+        <f>0.99*G61</f>
+        <v>0.84494520000000006</v>
       </c>
       <c r="D30" s="8">
         <f t="shared" si="4"/>
-        <v>8.4494520000000014E-3</v>
+        <v>0.84494520000000006</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>17</v>
@@ -1347,21 +1344,21 @@
     </row>
     <row r="31" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
       </c>
       <c r="C31" s="7">
-        <f>0.99*G62</f>
-        <v>0.84494520000000006</v>
+        <f>1.13/10*G61</f>
+        <v>9.644324E-2</v>
       </c>
       <c r="D31" s="8">
         <f t="shared" si="4"/>
-        <v>0.84494520000000006</v>
+        <v>9.644324E-2</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1372,15 +1369,15 @@
         <v>1</v>
       </c>
       <c r="C32" s="7">
-        <f>1.13/10*G62</f>
-        <v>9.644324E-2</v>
+        <f>0.84*G61/100</f>
+        <v>7.1692320000000002E-3</v>
       </c>
       <c r="D32" s="8">
         <f t="shared" si="4"/>
-        <v>9.644324E-2</v>
+        <v>7.1692320000000002E-3</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1391,12 +1388,12 @@
         <v>1</v>
       </c>
       <c r="C33" s="7">
-        <f>0.84*G62/100</f>
-        <v>7.1692320000000002E-3</v>
+        <f>0.96*G61/100</f>
+        <v>8.1934079999999992E-3</v>
       </c>
       <c r="D33" s="8">
         <f t="shared" si="4"/>
-        <v>7.1692320000000002E-3</v>
+        <v>8.1934079999999992E-3</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>17</v>
@@ -1404,95 +1401,87 @@
     </row>
     <row r="34" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B34" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="7">
-        <f>0.96*G62/100</f>
-        <v>8.1934079999999992E-3</v>
-      </c>
-      <c r="D34" s="8">
-        <f t="shared" si="4"/>
-        <v>8.1934079999999992E-3</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="6">
-        <v>2</v>
-      </c>
-      <c r="C35" s="7">
         <f>0.92/50</f>
         <v>1.84E-2</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D34" s="8">
         <f t="shared" si="4"/>
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="E34" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
     </row>
     <row r="37" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
+      <c r="A37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7">
+        <f>3.49*G61</f>
+        <v>2.9786452000000003</v>
+      </c>
+      <c r="D37" s="8">
+        <f>B37*C37</f>
+        <v>2.9786452000000003</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="7">
-        <f>3.49*G62</f>
-        <v>2.9786452000000003</v>
+        <f>4.42*G61</f>
+        <v>3.7723816000000001</v>
       </c>
       <c r="D38" s="8">
         <f>B38*C38</f>
-        <v>2.9786452000000003</v>
+        <v>7.5447632000000002</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>42</v>
+      <c r="A39" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="B39" s="6">
-        <v>2</v>
-      </c>
-      <c r="C39" s="7">
-        <f>4.42*G62</f>
-        <v>3.7723816000000001</v>
-      </c>
-      <c r="D39" s="8">
-        <f>B39*C39</f>
-        <v>7.5447632000000002</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>17</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
@@ -1506,118 +1495,126 @@
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>32</v>
+      <c r="A41" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="6">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="C41" s="7">
+        <f>1.38/50</f>
+        <v>2.76E-2</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" ref="D41:D42" si="5">B41*C41</f>
+        <v>0.1656</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B42" s="6">
         <v>6</v>
       </c>
       <c r="C42" s="7">
-        <f>1.38/50</f>
-        <v>2.76E-2</v>
-      </c>
-      <c r="D42" s="8">
-        <f t="shared" ref="D42:D43" si="5">B42*C42</f>
-        <v>0.1656</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="6">
-        <v>6</v>
-      </c>
-      <c r="C43" s="7">
         <f>4.61/500</f>
         <v>9.2200000000000008E-3</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D42" s="8">
         <f t="shared" si="5"/>
         <v>5.5320000000000008E-2</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="E42" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
+      <c r="A44" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="7">
+        <f>3.34*G61</f>
+        <v>2.8506231999999998</v>
+      </c>
+      <c r="D45" s="8">
+        <f t="shared" ref="D45:D48" si="6">B45*C45</f>
+        <v>2.8506231999999998</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="6">
-        <v>1</v>
-      </c>
-      <c r="C46" s="7">
-        <f>3.34*G62</f>
-        <v>2.8506231999999998</v>
-      </c>
-      <c r="D46" s="8">
-        <f t="shared" ref="D46:D49" si="6">B46*C46</f>
-        <v>2.8506231999999998</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
     </row>
     <row r="48" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
+      <c r="A48" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="7">
+        <v>12.66</v>
+      </c>
+      <c r="D48" s="8">
+        <f t="shared" si="6"/>
+        <v>12.66</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B49" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" s="7">
-        <v>12.66</v>
+        <f>1.09/50</f>
+        <v>2.18E-2</v>
       </c>
       <c r="D49" s="8">
-        <f t="shared" si="6"/>
-        <v>12.66</v>
+        <f>B49*C49</f>
+        <v>4.36E-2</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>18</v>
@@ -1625,18 +1622,18 @@
     </row>
     <row r="50" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B50" s="6">
         <v>2</v>
       </c>
       <c r="C50" s="7">
-        <f>1.09/50</f>
-        <v>2.18E-2</v>
+        <f>1.19/100</f>
+        <v>1.1899999999999999E-2</v>
       </c>
       <c r="D50" s="8">
         <f>B50*C50</f>
-        <v>4.36E-2</v>
+        <v>2.3799999999999998E-2</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>18</v>
@@ -1644,18 +1641,18 @@
     </row>
     <row r="51" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B51" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C51" s="7">
-        <f>1.19/100</f>
-        <v>1.1899999999999999E-2</v>
+        <f>1.38/50</f>
+        <v>2.76E-2</v>
       </c>
       <c r="D51" s="8">
-        <f>B51*C51</f>
-        <v>2.3799999999999998E-2</v>
+        <f t="shared" ref="D51:D53" si="7">B51*C51</f>
+        <v>0.1104</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>18</v>
@@ -1663,18 +1660,18 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B52" s="6">
         <v>4</v>
       </c>
       <c r="C52" s="7">
-        <f>1.38/50</f>
-        <v>2.76E-2</v>
+        <f>4.61/500</f>
+        <v>9.2200000000000008E-3</v>
       </c>
       <c r="D52" s="8">
-        <f t="shared" ref="D52:D54" si="7">B52*C52</f>
-        <v>0.1104</v>
+        <f t="shared" si="7"/>
+        <v>3.6880000000000003E-2</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>18</v>
@@ -1682,143 +1679,124 @@
     </row>
     <row r="53" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B53" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C53" s="7">
-        <f>4.61/500</f>
-        <v>9.2200000000000008E-3</v>
+        <f>0.99/8</f>
+        <v>0.12375</v>
       </c>
       <c r="D53" s="8">
         <f t="shared" si="7"/>
-        <v>3.6880000000000003E-2</v>
+        <v>0.12375</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>58</v>
+      <c r="A54" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="B54" s="6">
         <v>1</v>
       </c>
-      <c r="C54" s="7">
-        <f>0.99/8</f>
-        <v>0.12375</v>
-      </c>
-      <c r="D54" s="8">
-        <f t="shared" si="7"/>
-        <v>0.12375</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="6">
-        <v>1</v>
-      </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="9"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
+      <c r="A56" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
+      <c r="A57" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="6">
+        <v>1</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="D57" s="8">
+        <f>B57*C57</f>
+        <v>0.79</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B58" s="6">
         <v>1</v>
       </c>
       <c r="C58" s="7">
-        <v>0.79</v>
+        <v>6.15</v>
       </c>
       <c r="D58" s="8">
         <f>B58*C58</f>
-        <v>0.79</v>
+        <v>6.15</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="6">
-        <v>1</v>
-      </c>
-      <c r="C59" s="7">
-        <v>6.15</v>
-      </c>
-      <c r="D59" s="8">
-        <f>B59*C59</f>
-        <v>6.15</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="19"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="19"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="23"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="14">
+        <f>SUM(D3:D58)</f>
+        <v>89.750652802909087</v>
+      </c>
+      <c r="G60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="14">
-        <f>SUM(D3:D59)</f>
-        <v>89.750652802909087</v>
-      </c>
-      <c r="G61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D62" s="15">
+        <v>27</v>
+      </c>
+      <c r="D61" s="15">
         <f>13/1.1</f>
         <v>11.818181818181817</v>
       </c>
-      <c r="G62">
+      <c r="G61">
         <v>0.85348000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="13" t="s">
+    <row r="62" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="16">
-        <f>D61+D62</f>
+      <c r="D62" s="16">
+        <f>D60+D61</f>
         <v>101.5688346210909</v>
       </c>
     </row>
@@ -1828,50 +1806,49 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E59" r:id="rId5"/>
-    <hyperlink ref="E49" r:id="rId6"/>
-    <hyperlink ref="E39" r:id="rId7"/>
+    <hyperlink ref="E58" r:id="rId5"/>
+    <hyperlink ref="E48" r:id="rId6"/>
+    <hyperlink ref="E38" r:id="rId7"/>
     <hyperlink ref="E14" r:id="rId8"/>
     <hyperlink ref="E16" r:id="rId9"/>
     <hyperlink ref="E17" r:id="rId10"/>
-    <hyperlink ref="E32" r:id="rId11"/>
-    <hyperlink ref="E31" r:id="rId12"/>
-    <hyperlink ref="E35" r:id="rId13"/>
+    <hyperlink ref="E31" r:id="rId11"/>
+    <hyperlink ref="E30" r:id="rId12"/>
+    <hyperlink ref="E34" r:id="rId13"/>
     <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E46" r:id="rId15" display="Aliexpress"/>
-    <hyperlink ref="E38" r:id="rId16"/>
+    <hyperlink ref="E45" r:id="rId15" display="Aliexpress"/>
+    <hyperlink ref="E37" r:id="rId16"/>
     <hyperlink ref="E7" r:id="rId17"/>
-    <hyperlink ref="E58" r:id="rId18"/>
-    <hyperlink ref="E33" r:id="rId19"/>
-    <hyperlink ref="E34" r:id="rId20"/>
+    <hyperlink ref="E57" r:id="rId18"/>
+    <hyperlink ref="E32" r:id="rId19"/>
+    <hyperlink ref="E33" r:id="rId20"/>
     <hyperlink ref="E26" r:id="rId21"/>
-    <hyperlink ref="E27" r:id="rId22"/>
-    <hyperlink ref="E25" r:id="rId23"/>
-    <hyperlink ref="E24" r:id="rId24"/>
-    <hyperlink ref="E18" r:id="rId25"/>
-    <hyperlink ref="E13" r:id="rId26"/>
+    <hyperlink ref="E25" r:id="rId22"/>
+    <hyperlink ref="E24" r:id="rId23"/>
+    <hyperlink ref="E18" r:id="rId24"/>
+    <hyperlink ref="E13" r:id="rId25"/>
+    <hyperlink ref="E27" r:id="rId26"/>
     <hyperlink ref="E28" r:id="rId27"/>
     <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E21" r:id="rId30"/>
-    <hyperlink ref="E23" r:id="rId31"/>
+    <hyperlink ref="E21" r:id="rId29"/>
+    <hyperlink ref="E23" r:id="rId30"/>
+    <hyperlink ref="E49" r:id="rId31"/>
     <hyperlink ref="E50" r:id="rId32"/>
-    <hyperlink ref="E51" r:id="rId33"/>
-    <hyperlink ref="E43" r:id="rId34"/>
-    <hyperlink ref="E53" r:id="rId35"/>
-    <hyperlink ref="E12" r:id="rId36"/>
-    <hyperlink ref="E10" r:id="rId37"/>
-    <hyperlink ref="E9" r:id="rId38"/>
-    <hyperlink ref="E42" r:id="rId39"/>
-    <hyperlink ref="E52" r:id="rId40"/>
-    <hyperlink ref="E11" r:id="rId41"/>
-    <hyperlink ref="E22" r:id="rId42"/>
-    <hyperlink ref="E19" r:id="rId43"/>
-    <hyperlink ref="E54" r:id="rId44"/>
-    <hyperlink ref="E20" r:id="rId45"/>
+    <hyperlink ref="E42" r:id="rId33"/>
+    <hyperlink ref="E52" r:id="rId34"/>
+    <hyperlink ref="E12" r:id="rId35"/>
+    <hyperlink ref="E10" r:id="rId36"/>
+    <hyperlink ref="E9" r:id="rId37"/>
+    <hyperlink ref="E41" r:id="rId38"/>
+    <hyperlink ref="E51" r:id="rId39"/>
+    <hyperlink ref="E11" r:id="rId40"/>
+    <hyperlink ref="E22" r:id="rId41"/>
+    <hyperlink ref="E19" r:id="rId42"/>
+    <hyperlink ref="E53" r:id="rId43"/>
+    <hyperlink ref="E20" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId45"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
     <ignoredError sqref="C11" formula="1"/>

</xml_diff>